<commit_message>
manager table and colours
</commit_message>
<xml_diff>
--- a/media/files/colours.xlsx
+++ b/media/files/colours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afb61024139a389c/Hobbies/Django/Skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{31324D30-D7C1-4A09-B5CF-DE4C6FA6FCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EE0152C-5C59-41DF-ADC0-EBD86C6F575C}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{31324D30-D7C1-4A09-B5CF-DE4C6FA6FCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74E45714-053A-4ECF-8283-CE5896CAF7D4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C09C7F88-4454-4448-A43D-DDD3083C754F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>AC97CC</t>
   </si>
@@ -87,10 +87,73 @@
     <t>FDFFB6</t>
   </si>
   <si>
-    <t>BDB2FF</t>
-  </si>
-  <si>
     <t>Calm</t>
+  </si>
+  <si>
+    <t>2a9d8f</t>
+  </si>
+  <si>
+    <t>e9c46a</t>
+  </si>
+  <si>
+    <t>f4a261</t>
+  </si>
+  <si>
+    <t>e76f51</t>
+  </si>
+  <si>
+    <t>Green and Gold</t>
+  </si>
+  <si>
+    <t>fec5bb</t>
+  </si>
+  <si>
+    <t>fcd5ce</t>
+  </si>
+  <si>
+    <t>fec89a</t>
+  </si>
+  <si>
+    <t>ffd7ba</t>
+  </si>
+  <si>
+    <t>Pastel</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>03045e</t>
+  </si>
+  <si>
+    <t>023e8a</t>
+  </si>
+  <si>
+    <t>0077b6</t>
+  </si>
+  <si>
+    <t>48cae4</t>
+  </si>
+  <si>
+    <t>90e0ef</t>
+  </si>
+  <si>
+    <t>184E77</t>
+  </si>
+  <si>
+    <t>1e6091</t>
+  </si>
+  <si>
+    <t>1a759f</t>
+  </si>
+  <si>
+    <t>d9ed92</t>
+  </si>
+  <si>
+    <t>b5e48c</t>
+  </si>
+  <si>
+    <t>Blue and Green</t>
   </si>
 </sst>
 </file>
@@ -126,8 +189,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,14 +507,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2F25A7-C0F1-4AE0-8908-3C5BA9862154}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
@@ -504,13 +570,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -523,6 +589,98 @@
       </c>
       <c r="G3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>264653</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>791402</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>